<commit_message>
Fixed images and instructions for README-Alexa
</commit_message>
<xml_diff>
--- a/VPA_Reinvent_Tasks.xlsx
+++ b/VPA_Reinvent_Tasks.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="80">
   <si>
     <t>Item</t>
   </si>
@@ -264,12 +264,36 @@
   <si>
     <t>Athena Step 2 Partial</t>
   </si>
+  <si>
+    <t>https://github.com/voicehacks/setup-local-recommendations/blob/master/speech-assets/InteractionModel.json</t>
+  </si>
+  <si>
+    <t>50% complete</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Split out Athena from Main README</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>Done form Alexa</t>
+  </si>
+  <si>
+    <t>Need to validate</t>
+  </si>
+  <si>
+    <t>20% completed</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -281,6 +305,12 @@
       <sz val="12"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Menlo"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -303,8 +333,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -582,10 +614,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E41"/>
+  <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -595,7 +627,7 @@
     <col min="3" max="3" width="65.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -611,19 +643,25 @@
       <c r="E1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="C2" t="s">
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="E2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+        <v>76</v>
+      </c>
+      <c r="F2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -637,7 +675,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>71</v>
       </c>
@@ -651,7 +689,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -662,10 +700,13 @@
         <v>24</v>
       </c>
       <c r="E5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+        <v>73</v>
+      </c>
+      <c r="F5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>42</v>
       </c>
@@ -679,7 +720,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -693,7 +734,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>30</v>
       </c>
@@ -707,7 +748,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>30</v>
       </c>
@@ -718,10 +759,13 @@
         <v>14</v>
       </c>
       <c r="E9" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+        <v>73</v>
+      </c>
+      <c r="F9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>42</v>
       </c>
@@ -735,7 +779,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -749,7 +793,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>30</v>
       </c>
@@ -763,7 +807,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -777,7 +821,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -788,10 +832,13 @@
         <v>14</v>
       </c>
       <c r="E14" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+        <v>73</v>
+      </c>
+      <c r="F14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -802,10 +849,10 @@
         <v>14</v>
       </c>
       <c r="E15" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>19</v>
       </c>
@@ -817,6 +864,9 @@
       </c>
       <c r="E16" t="s">
         <v>25</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
@@ -854,8 +904,8 @@
       <c r="D19" t="s">
         <v>14</v>
       </c>
-      <c r="E19" t="s">
-        <v>25</v>
+      <c r="E19" s="2" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
@@ -953,7 +1003,7 @@
         <v>14</v>
       </c>
       <c r="E26" t="s">
-        <v>25</v>
+        <v>76</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
@@ -1081,7 +1131,7 @@
         <v>61</v>
       </c>
       <c r="D36" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="E36" t="s">
         <v>25</v>

</xml_diff>

<commit_message>
Working on Athena README
</commit_message>
<xml_diff>
--- a/VPA_Reinvent_Tasks.xlsx
+++ b/VPA_Reinvent_Tasks.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28702"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28810"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/awwestri/Documents/vpa/Github/voice-powered-analytics/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chadneal/code/voice-powered-analytics/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-35960" yWindow="3700" windowWidth="24960" windowHeight="13460" tabRatio="500"/>
+    <workbookView xWindow="1480" yWindow="2340" windowWidth="24960" windowHeight="13460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="78">
   <si>
     <t>Item</t>
   </si>
@@ -278,6 +278,9 @@
   </si>
   <si>
     <t>Add environment variable for metric intent. Default: WhatsMyMetric</t>
+  </si>
+  <si>
+    <t>done</t>
   </si>
 </sst>
 </file>
@@ -638,13 +641,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.6640625" customWidth="1"/>
     <col min="2" max="2" width="17.1640625" customWidth="1"/>
     <col min="3" max="3" width="65.6640625" bestFit="1" customWidth="1"/>
   </cols>
@@ -694,7 +697,7 @@
         <v>18</v>
       </c>
       <c r="E3" t="s">
-        <v>23</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -708,7 +711,7 @@
         <v>18</v>
       </c>
       <c r="E4" t="s">
-        <v>23</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -963,7 +966,7 @@
         <v>18</v>
       </c>
       <c r="E22" t="s">
-        <v>23</v>
+        <v>73</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>